<commit_message>
added laptop benchmarks and serial flag -s
</commit_message>
<xml_diff>
--- a/Project/benchmark_data/benchmark.xlsx
+++ b/Project/benchmark_data/benchmark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Uni\Algorithm-Engineering\Project\benchmark_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Uni\Algorithm Engineering\Project\benchmark_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EF5E5C1-8A47-41A4-9F8C-76D5F323BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9E32E04-3D0F-4659-8274-D2F738380D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{47E42F5F-413F-444C-A1C5-791889E20C66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{47E42F5F-413F-444C-A1C5-791889E20C66}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="167" formatCode="0.000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,12 +98,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -116,7 +120,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,16 +439,16 @@
   <dimension ref="C3:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -461,17 +465,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.45508799999999999</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>5.6426999999999998E-2</v>
       </c>
       <c r="G4" s="1">
@@ -479,17 +483,17 @@
         <v>8.0650752299431119</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
         <v>50</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>2.7025960000000002</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>0.24926100000000001</v>
       </c>
       <c r="G5" s="1">
@@ -497,17 +501,17 @@
         <v>10.842434235600436</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>1</v>
       </c>
       <c r="D6">
         <v>100</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>10.915958</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>1.030694</v>
       </c>
       <c r="G6" s="1">
@@ -515,17 +519,17 @@
         <v>10.590881483738141</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7">
         <v>20</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>1.327925</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>0.15176600000000001</v>
       </c>
       <c r="G7" s="1">
@@ -533,17 +537,17 @@
         <v>8.7498187999947277</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8">
         <v>50</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>7.8141720000000001</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>0.70990399999999998</v>
       </c>
       <c r="G8" s="1">
@@ -551,17 +555,17 @@
         <v>11.007364376028308</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>2</v>
       </c>
       <c r="D9">
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>31.977059000000001</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>3.037814</v>
       </c>
       <c r="G9" s="1">
@@ -569,129 +573,132 @@
         <v>10.526338676429827</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="G11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>1</v>
       </c>
       <c r="D12">
         <v>20</v>
       </c>
-      <c r="E12">
-        <v>0.45508799999999999</v>
-      </c>
-      <c r="F12">
-        <v>5.6426999999999998E-2</v>
+      <c r="E12" s="2">
+        <v>0.34914800000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <v>8.7414000000000006E-2</v>
       </c>
       <c r="G12" s="1">
         <f>E12/F12</f>
-        <v>8.0650752299431119</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+        <v>3.9941885739126453</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13">
         <v>50</v>
       </c>
-      <c r="E13">
-        <v>2.7025960000000002</v>
-      </c>
-      <c r="F13">
+      <c r="E13" s="2">
+        <v>1.9693670000000001</v>
+      </c>
+      <c r="F13" s="2">
         <v>0.24926100000000001</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G17" si="1">E13/F13</f>
-        <v>10.842434235600436</v>
-      </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+        <v>0.359487</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>1</v>
       </c>
       <c r="D14">
         <v>100</v>
       </c>
-      <c r="E14">
-        <v>10.915958</v>
-      </c>
-      <c r="F14">
-        <v>1.030694</v>
+      <c r="E14" s="2">
+        <v>7.500394</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1.363164</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
-        <v>10.590881483738141</v>
-      </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+        <f t="shared" ref="G13:G17" si="1">E14/F14</f>
+        <v>5.502194893644492</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>2</v>
       </c>
       <c r="D15">
         <v>20</v>
       </c>
-      <c r="E15">
-        <v>1.327925</v>
-      </c>
-      <c r="F15">
-        <v>0.15176600000000001</v>
+      <c r="E15" s="2">
+        <v>1.0436350000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.201269</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>8.7498187999947277</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+        <v>5.1852744337180594</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16">
         <v>50</v>
       </c>
-      <c r="E16">
-        <v>7.8141720000000001</v>
-      </c>
-      <c r="F16">
-        <v>0.70990399999999998</v>
+      <c r="E16" s="2">
+        <v>5.9694089999999997</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.98385299999999998</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>11.007364376028308</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+        <v>6.0673789681995176</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>2</v>
       </c>
       <c r="D17">
         <v>100</v>
       </c>
-      <c r="E17">
-        <v>31.977059000000001</v>
-      </c>
-      <c r="F17">
-        <v>3.037814</v>
+      <c r="E17" s="2">
+        <v>22.801159999999999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>3.6349140000000002</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>10.526338676429827</v>
+        <v>6.2728196595572818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>